<commit_message>
bf: update the form
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Burkina Faso/bf_oncho_pre_stop_2_202312_couverture.xlsx
+++ b/ONCHO/Impact Assessments/Burkina Faso/bf_oncho_pre_stop_2_202312_couverture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Burkina Faso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389D8D0F-2ABA-49DF-89CB-AAF7403D583E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCABC36-FA6C-4FEC-8529-8612A71E7293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="188">
   <si>
     <t>type</t>
   </si>
@@ -594,6 +594,9 @@
   </si>
   <si>
     <t>regex(., '^[0-9]{2}$') and .&lt;100 and (not(selected(${C3}, ${Numero_enquete})))</t>
+  </si>
+  <si>
+    <t>${Recu_IVM} = 'Oui' and ${consentement} = 'Oui'</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1049,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,7 +1421,7 @@
         <v>160</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
bf: update participant form.
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Burkina Faso/bf_oncho_pre_stop_2_202312_couverture.xlsx
+++ b/ONCHO/Impact Assessments/Burkina Faso/bf_oncho_pre_stop_2_202312_couverture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Burkina Faso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCABC36-FA6C-4FEC-8529-8612A71E7293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45838986-E770-4DB3-8792-940DF1815805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -560,15 +560,6 @@
     <t>Le code doit avoir deux chiffre et être utilisé une seul fois par foyer.</t>
   </si>
   <si>
-    <t>p_bf_202312_1</t>
-  </si>
-  <si>
-    <t>(Dec 2023) ONCHO - 2. Formulaire Enrolement V1</t>
-  </si>
-  <si>
-    <t>bf_oncho_pre_stop_2_202312_couverture_v1</t>
-  </si>
-  <si>
     <t>consentement</t>
   </si>
   <si>
@@ -597,6 +588,15 @@
   </si>
   <si>
     <t>${Recu_IVM} = 'Oui' and ${consentement} = 'Oui'</t>
+  </si>
+  <si>
+    <t>(Dec 2023) ONCHO - 2. Formulaire Enrolement V2</t>
+  </si>
+  <si>
+    <t>bf_oncho_pre_stop_2_202312_couverture_v2</t>
+  </si>
+  <si>
+    <t>p_bf_202312_2</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1049,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,10 +1212,10 @@
         <v>168</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -1256,10 +1256,10 @@
         <v>47</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I12" s="7"/>
     </row>
@@ -1274,13 +1274,13 @@
         <v>41</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>174</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>15</v>
@@ -1300,7 +1300,7 @@
         <v>64</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>15</v>
@@ -1329,7 +1329,7 @@
         <v>65</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>15</v>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="E16" s="8"/>
       <c r="H16" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>15</v>
@@ -1364,7 +1364,7 @@
         <v>157</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>15</v>
@@ -1387,7 +1387,7 @@
         <v>66</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>15</v>
@@ -1404,7 +1404,7 @@
         <v>159</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>15</v>
@@ -1421,7 +1421,7 @@
         <v>160</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>15</v>
@@ -1438,7 +1438,7 @@
         <v>161</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I21" s="7" t="s">
         <v>15</v>
@@ -1455,7 +1455,7 @@
         <v>162</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>15</v>
@@ -1472,7 +1472,7 @@
         <v>163</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>15</v>
@@ -1492,40 +1492,40 @@
         <v>67</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
@@ -2196,10 +2196,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>19</v>

</xml_diff>